<commit_message>
2 insertions to db
</commit_message>
<xml_diff>
--- a/inst/db/cmvdrg-db1.xlsx
+++ b/inst/db/cmvdrg-db1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Oscar\OneDrive\UCL\complete\19-6_cmvdrg\cmvdrg\inst\db\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85376FD3-1931-458C-8CF7-2BA0708D19C0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D45299A9-25B7-4AA9-8674-C88A13DC7143}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="390" yWindow="390" windowWidth="28800" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="cmvdrg-db1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6399" uniqueCount="773">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6423" uniqueCount="778">
   <si>
     <t>Letermovir</t>
   </si>
@@ -2402,6 +2402,23 @@
   </si>
   <si>
     <t>DOI: 10.1128/JVI.01787-07</t>
+  </si>
+  <si>
+    <t>Q579I</t>
+  </si>
+  <si>
+    <t>0.16</t>
+  </si>
+  <si>
+    <t>Hypersusceptibility of Human Cytomegalovirus to Foscarnet
+Induced by Mutations in Helices K and P of the Viral DNA
+Polymerase</t>
+  </si>
+  <si>
+    <t>https://aac.asm.org/content/aac/64/4/e01910-19.full.pdf</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1128/AAC.01910-19</t>
   </si>
 </sst>
 </file>
@@ -3860,11 +3877,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z577"/>
+  <dimension ref="A1:Z579"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A250" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K264" sqref="K264"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A542" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H583" sqref="H583"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3875,7 +3892,7 @@
     <col min="7" max="13" width="9.140625" customWidth="1"/>
     <col min="19" max="19" width="18.5703125" customWidth="1"/>
     <col min="20" max="20" width="10.85546875" customWidth="1"/>
-    <col min="23" max="23" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="13" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" x14ac:dyDescent="0.25">
@@ -30070,6 +30087,100 @@
         <v>10</v>
       </c>
       <c r="Z577" t="s">
+        <v>670</v>
+      </c>
+    </row>
+    <row r="578" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A578">
+        <v>580</v>
+      </c>
+      <c r="B578" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C578" t="s">
+        <v>353</v>
+      </c>
+      <c r="D578" t="s">
+        <v>6</v>
+      </c>
+      <c r="E578" t="s">
+        <v>773</v>
+      </c>
+      <c r="F578" s="18" t="s">
+        <v>774</v>
+      </c>
+      <c r="H578">
+        <v>0.06</v>
+      </c>
+      <c r="P578" s="6" t="s">
+        <v>775</v>
+      </c>
+      <c r="Q578" s="2" t="s">
+        <v>776</v>
+      </c>
+      <c r="R578" t="s">
+        <v>777</v>
+      </c>
+      <c r="S578" t="s">
+        <v>506</v>
+      </c>
+      <c r="T578" t="s">
+        <v>9</v>
+      </c>
+      <c r="W578" s="1">
+        <v>44034</v>
+      </c>
+      <c r="X578" t="s">
+        <v>10</v>
+      </c>
+      <c r="Z578" t="s">
+        <v>670</v>
+      </c>
+    </row>
+    <row r="579" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A579">
+        <v>580</v>
+      </c>
+      <c r="B579" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C579" t="s">
+        <v>353</v>
+      </c>
+      <c r="D579" t="s">
+        <v>6</v>
+      </c>
+      <c r="E579" t="s">
+        <v>77</v>
+      </c>
+      <c r="F579" s="18" t="s">
+        <v>695</v>
+      </c>
+      <c r="H579">
+        <v>0.19</v>
+      </c>
+      <c r="P579" s="6" t="s">
+        <v>775</v>
+      </c>
+      <c r="Q579" s="2" t="s">
+        <v>776</v>
+      </c>
+      <c r="R579" t="s">
+        <v>777</v>
+      </c>
+      <c r="S579" t="s">
+        <v>506</v>
+      </c>
+      <c r="T579" t="s">
+        <v>9</v>
+      </c>
+      <c r="W579" s="1">
+        <v>44034</v>
+      </c>
+      <c r="X579" t="s">
+        <v>10</v>
+      </c>
+      <c r="Z579" t="s">
         <v>670</v>
       </c>
     </row>
@@ -30901,8 +31012,10 @@
     <hyperlink ref="Q288" r:id="rId663" xr:uid="{3183101C-BB39-4312-A080-BCD82DE9AB29}"/>
     <hyperlink ref="Q285" r:id="rId664" xr:uid="{4061A7FF-0E94-4C8F-AE28-F48E2C895554}"/>
     <hyperlink ref="R285" r:id="rId665" xr:uid="{0D93EDC8-4345-4A05-8FFB-1D4CEE08EC02}"/>
+    <hyperlink ref="Q578" r:id="rId666" xr:uid="{4303DE3C-6972-4511-9ACC-3F11D6D80A54}"/>
+    <hyperlink ref="Q579" r:id="rId667" xr:uid="{2C7A021C-8BC4-4978-B230-42CBF5D527E7}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId666"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId668"/>
 </worksheet>
 </file>
</xml_diff>